<commit_message>
Changed filenames for each algo to correct ones
</commit_message>
<xml_diff>
--- a/ex_nr_ex2.xlsx
+++ b/ex_nr_ex2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uxue\Desktop\TETE4205\PowerFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C26C5F-7932-8148-A232-B033BCC0B40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FAE9CA-1E9A-4BF6-B041-A0675722E637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="20920" windowHeight="14320" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
+    <workbookView xWindow="-28920" yWindow="-1095" windowWidth="29040" windowHeight="17520" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -28,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -88,9 +86,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -117,8 +122,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,15 +443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CC4DDF-8E3E-324E-AB44-8876A263AA5F}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,39 +474,69 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.14669763999999999</v>
+      </c>
       <c r="E3">
         <v>1.63</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4.5319579999999998E-2</v>
+      </c>
       <c r="E4">
         <v>0.85</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-4.1805630000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-8.4627740000000007E-2</v>
+      </c>
       <c r="E6">
         <v>-1.25</v>
       </c>
@@ -504,10 +544,16 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-0.13192544</v>
+      </c>
       <c r="E7">
         <v>-0.9</v>
       </c>
@@ -515,15 +561,27 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4.4822639999999997E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-1.845047E-2</v>
+      </c>
       <c r="E9">
         <v>-1</v>
       </c>
@@ -531,13 +589,23 @@
         <v>-0.35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-4.4904200000000002E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -549,9 +617,9 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -574,7 +642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>78</v>
       </c>
@@ -591,7 +659,7 @@
         <v>7.4499999999999997E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>89</v>
       </c>
@@ -608,7 +676,7 @@
         <v>0.1045</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>75</v>
       </c>
@@ -625,7 +693,7 @@
         <v>0.153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>96</v>
       </c>
@@ -642,7 +710,7 @@
         <v>0.17899999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>54</v>
       </c>
@@ -659,7 +727,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>64</v>
       </c>
@@ -676,7 +744,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>14</v>
       </c>
@@ -688,7 +756,7 @@
         <v>7.1739130434782611E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>27</v>
       </c>
@@ -700,7 +768,7 @@
         <v>7.8260869565217397E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Added description to DCPF and changed ex2 excel file with pv and pq
</commit_message>
<xml_diff>
--- a/ex_nr_ex2.xlsx
+++ b/ex_nr_ex2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ximena\Desktop\project tet4205\PowerFlow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uxue\Desktop\TETE4205\PowerFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D065FAE0-55E9-4848-8B49-37462FB1B578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D883CCA-12AE-4D82-B836-D521A5EC4F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2540" yWindow="1340" windowWidth="13290" windowHeight="8430" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -128,12 +128,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,15 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CC4DDF-8E3E-324E-AB44-8876A263AA5F}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,78 +480,50 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.14669763999999999</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3">
         <v>1.63</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>4.5319579999999998E-2</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4">
         <v>0.85</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>-4.1805630000000003E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>-8.4627740000000007E-2</v>
-      </c>
       <c r="E6">
         <v>-1.25</v>
       </c>
@@ -558,19 +531,13 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>-0.13192544</v>
-      </c>
       <c r="E7">
         <v>-0.9</v>
       </c>
@@ -578,30 +545,18 @@
         <v>-0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>4.4822639999999997E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>-1.845047E-2</v>
-      </c>
       <c r="E9">
         <v>-1</v>
       </c>
@@ -609,16 +564,13 @@
         <v>-0.35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>-4.4904200000000002E-3</v>
-      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -634,9 +586,9 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -659,7 +611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>78</v>
       </c>
@@ -676,7 +628,7 @@
         <v>7.4499999999999997E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>89</v>
       </c>
@@ -693,7 +645,7 @@
         <v>0.1045</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>75</v>
       </c>
@@ -710,7 +662,7 @@
         <v>0.153</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>96</v>
       </c>
@@ -727,7 +679,7 @@
         <v>0.17899999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>54</v>
       </c>
@@ -744,7 +696,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>64</v>
       </c>
@@ -761,7 +713,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>14</v>
       </c>
@@ -773,7 +725,7 @@
         <v>7.1739130434782611E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>27</v>
       </c>
@@ -785,7 +737,7 @@
         <v>7.8260869565217397E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>39</v>
       </c>

</xml_diff>